<commit_message>
Updated Examples using Selfweights
</commit_message>
<xml_diff>
--- a/Examples/GUI_Truss2D/GUI_Arch Truss_1.xlsx
+++ b/Examples/GUI_Truss2D/GUI_Arch Truss_1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdc3a34d3e00f8dc/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xelonix\Documents\_Github\pysead\Examples\GUI_Truss2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_98B1FBEB28D2CA068DEAD27991DB0C10CA837A9E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D58DA267-4B5A-46D8-BD44-749519FFF9A1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B3BE37-E9EB-4675-9944-A2E942C76269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nodes" sheetId="1" r:id="rId1"/>
-    <sheet name="Elements" sheetId="2" r:id="rId2"/>
+    <sheet name="Elements" sheetId="2" r:id="rId1"/>
+    <sheet name="Nodes" sheetId="1" r:id="rId2"/>
     <sheet name="Materials" sheetId="3" r:id="rId3"/>
     <sheet name="Supports" sheetId="4" r:id="rId4"/>
     <sheet name="Load_Cases" sheetId="5" r:id="rId5"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>Node</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>F_y</t>
+  </si>
+  <si>
+    <t>self-weight</t>
   </si>
 </sst>
 </file>
@@ -443,22 +446,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -469,10 +474,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-7.8</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -483,10 +488,10 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>-7.4249999999999998</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -497,10 +502,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>7.4249999999999998</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -511,10 +516,10 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>7.8</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -525,10 +530,10 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>-7.8</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -539,10 +544,10 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>-7.4249999999999998</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -553,10 +558,10 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>7.4249999999999998</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -567,10 +572,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>7.8</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -581,10 +586,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>-7.4265999999999996</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>1.6267</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -595,10 +600,10 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>7.4265999999999996</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>1.6267</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -609,10 +614,10 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>-7.8</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>1.65</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,10 +628,10 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>7.8</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>1.65</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -637,10 +642,10 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>-7.4281999999999986</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>2.7532999999999999</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -651,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>7.4281999999999986</v>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>2.7532999999999999</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -665,10 +670,10 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>-7.8</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>2.8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -679,10 +684,10 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>7.8</v>
+        <v>8</v>
       </c>
       <c r="D17">
-        <v>2.8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -693,10 +698,10 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>-7.2062999999999997</v>
+        <v>11</v>
       </c>
       <c r="D18">
-        <v>3.4849000000000001</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -707,10 +712,10 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>7.2062999999999997</v>
+        <v>10</v>
       </c>
       <c r="D19">
-        <v>3.4849000000000001</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -721,10 +726,10 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <v>-7.8</v>
+        <v>9</v>
       </c>
       <c r="D20">
-        <v>3.95</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,10 +740,10 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>7.8</v>
+        <v>10</v>
       </c>
       <c r="D21">
-        <v>3.95</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -749,10 +754,10 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <v>-6.8459000000000003</v>
+        <v>9</v>
       </c>
       <c r="D22">
-        <v>4.1592000000000002</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -763,10 +768,10 @@
         <v>22</v>
       </c>
       <c r="C23">
-        <v>6.8458999999999994</v>
+        <v>10</v>
       </c>
       <c r="D23">
-        <v>4.1592000000000002</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -777,10 +782,10 @@
         <v>23</v>
       </c>
       <c r="C24">
-        <v>-6.4855</v>
+        <v>11</v>
       </c>
       <c r="D24">
-        <v>4.8334999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -791,10 +796,10 @@
         <v>24</v>
       </c>
       <c r="C25">
-        <v>6.4855000000000009</v>
+        <v>12</v>
       </c>
       <c r="D25">
-        <v>4.8334999999999999</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -805,10 +810,10 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>-7.8</v>
+        <v>15</v>
       </c>
       <c r="D26">
-        <v>5.0999999999999996</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,10 +824,10 @@
         <v>26</v>
       </c>
       <c r="C27">
-        <v>7.8</v>
+        <v>16</v>
       </c>
       <c r="D27">
-        <v>5.0999999999999996</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -833,10 +838,10 @@
         <v>27</v>
       </c>
       <c r="C28">
-        <v>-5.9371</v>
+        <v>13</v>
       </c>
       <c r="D28">
-        <v>5.5015999999999998</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -847,10 +852,10 @@
         <v>28</v>
       </c>
       <c r="C29">
-        <v>5.9371</v>
+        <v>14</v>
       </c>
       <c r="D29">
-        <v>5.5015999999999998</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,10 +866,10 @@
         <v>29</v>
       </c>
       <c r="C30">
-        <v>-7.8</v>
+        <v>17</v>
       </c>
       <c r="D30">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -875,10 +880,10 @@
         <v>30</v>
       </c>
       <c r="C31">
-        <v>7.8</v>
+        <v>18</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,10 +894,10 @@
         <v>31</v>
       </c>
       <c r="C32">
-        <v>-5.5153999999999996</v>
+        <v>15</v>
       </c>
       <c r="D32">
-        <v>6.0153999999999996</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -903,10 +908,10 @@
         <v>32</v>
       </c>
       <c r="C33">
-        <v>5.5154000000000014</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>6.0153999999999996</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -917,10 +922,10 @@
         <v>33</v>
       </c>
       <c r="C34">
-        <v>-4.9851999999999999</v>
+        <v>19</v>
       </c>
       <c r="D34">
-        <v>6.4505999999999997</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -931,10 +936,10 @@
         <v>34</v>
       </c>
       <c r="C35">
-        <v>4.9851999999999999</v>
+        <v>20</v>
       </c>
       <c r="D35">
-        <v>6.4505999999999997</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -945,10 +950,10 @@
         <v>35</v>
       </c>
       <c r="C36">
-        <v>-7.1082000000000001</v>
+        <v>21</v>
       </c>
       <c r="D36">
-        <v>6.4625000000000004</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -959,10 +964,10 @@
         <v>36</v>
       </c>
       <c r="C37">
-        <v>7.1080999999999994</v>
+        <v>18</v>
       </c>
       <c r="D37">
-        <v>6.4626000000000001</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,10 +978,10 @@
         <v>37</v>
       </c>
       <c r="C38">
-        <v>-6.3889999999999993</v>
+        <v>25</v>
       </c>
       <c r="D38">
-        <v>6.8813000000000004</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,10 +992,10 @@
         <v>38</v>
       </c>
       <c r="C39">
-        <v>6.3888999999999996</v>
+        <v>26</v>
       </c>
       <c r="D39">
-        <v>6.8814000000000002</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1001,10 +1006,10 @@
         <v>39</v>
       </c>
       <c r="C40">
-        <v>-4.3333999999999993</v>
+        <v>23</v>
       </c>
       <c r="D40">
-        <v>6.9855</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1015,10 +1020,10 @@
         <v>40</v>
       </c>
       <c r="C41">
-        <v>4.3334000000000001</v>
+        <v>22</v>
       </c>
       <c r="D41">
-        <v>6.9855</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1029,10 +1034,10 @@
         <v>41</v>
       </c>
       <c r="C42">
-        <v>-5.6452</v>
+        <v>19</v>
       </c>
       <c r="D42">
-        <v>7.2546999999999997</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,10 +1048,10 @@
         <v>42</v>
       </c>
       <c r="C43">
-        <v>5.6451000000000002</v>
+        <v>20</v>
       </c>
       <c r="D43">
-        <v>7.2546999999999997</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,10 +1062,10 @@
         <v>43</v>
       </c>
       <c r="C44">
-        <v>-3.7848000000000002</v>
+        <v>25</v>
       </c>
       <c r="D44">
-        <v>7.2786999999999997</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1071,10 +1076,10 @@
         <v>44</v>
       </c>
       <c r="C45">
-        <v>3.7848000000000002</v>
+        <v>26</v>
       </c>
       <c r="D45">
-        <v>7.2786999999999997</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1085,10 +1090,10 @@
         <v>45</v>
       </c>
       <c r="C46">
-        <v>-4.8796999999999997</v>
+        <v>25</v>
       </c>
       <c r="D46">
-        <v>7.5812999999999997</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1099,10 +1104,10 @@
         <v>46</v>
       </c>
       <c r="C47">
-        <v>4.8796000000000008</v>
+        <v>24</v>
       </c>
       <c r="D47">
-        <v>7.5812999999999997</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,10 +1118,10 @@
         <v>47</v>
       </c>
       <c r="C48">
-        <v>-2.9849000000000001</v>
+        <v>27</v>
       </c>
       <c r="D48">
-        <v>7.7062999999999997</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1127,10 +1132,10 @@
         <v>48</v>
       </c>
       <c r="C49">
-        <v>2.984900000000001</v>
+        <v>24</v>
       </c>
       <c r="D49">
-        <v>7.7062999999999997</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1141,10 +1146,10 @@
         <v>49</v>
       </c>
       <c r="C50">
-        <v>-4.0953999999999997</v>
+        <v>29</v>
       </c>
       <c r="D50">
-        <v>7.8597000000000001</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1155,10 +1160,10 @@
         <v>50</v>
       </c>
       <c r="C51">
-        <v>4.0954000000000006</v>
+        <v>30</v>
       </c>
       <c r="D51">
-        <v>7.8597000000000001</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1169,10 +1174,10 @@
         <v>51</v>
       </c>
       <c r="C52">
-        <v>-2.3689</v>
+        <v>25</v>
       </c>
       <c r="D52">
-        <v>7.8930999999999996</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1183,10 +1188,10 @@
         <v>52</v>
       </c>
       <c r="C53">
-        <v>2.3689000000000009</v>
+        <v>26</v>
       </c>
       <c r="D53">
-        <v>7.8930999999999996</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1197,10 +1202,10 @@
         <v>53</v>
       </c>
       <c r="C54">
-        <v>-3.2953999999999999</v>
+        <v>35</v>
       </c>
       <c r="D54">
-        <v>8.0890000000000004</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1211,10 +1216,10 @@
         <v>54</v>
       </c>
       <c r="C55">
-        <v>3.2953999999999999</v>
+        <v>36</v>
       </c>
       <c r="D55">
-        <v>8.0891000000000002</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1225,10 +1230,10 @@
         <v>55</v>
       </c>
       <c r="C56">
-        <v>-1.5217000000000001</v>
+        <v>31</v>
       </c>
       <c r="D56">
-        <v>8.1501000000000001</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1239,10 +1244,10 @@
         <v>56</v>
       </c>
       <c r="C57">
-        <v>1.5217000000000001</v>
+        <v>28</v>
       </c>
       <c r="D57">
-        <v>8.1501000000000001</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1253,10 +1258,10 @@
         <v>57</v>
       </c>
       <c r="C58">
-        <v>-0.80679999999999996</v>
+        <v>35</v>
       </c>
       <c r="D58">
-        <v>8.2204999999999995</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,10 +1272,10 @@
         <v>58</v>
       </c>
       <c r="C59">
-        <v>0.80679999999999996</v>
+        <v>36</v>
       </c>
       <c r="D59">
-        <v>8.2204999999999995</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1281,10 +1286,10 @@
         <v>59</v>
       </c>
       <c r="C60">
-        <v>-2.482699999999999</v>
+        <v>29</v>
       </c>
       <c r="D60">
-        <v>8.2683</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1295,10 +1300,10 @@
         <v>60</v>
       </c>
       <c r="C61">
-        <v>2.4826999999999999</v>
+        <v>36</v>
       </c>
       <c r="D61">
-        <v>8.2683</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1309,10 +1314,10 @@
         <v>61</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D62">
-        <v>8.3000000000000007</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1323,10 +1328,10 @@
         <v>62</v>
       </c>
       <c r="C63">
-        <v>-1.6605000000000001</v>
+        <v>32</v>
       </c>
       <c r="D63">
-        <v>8.3969000000000005</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1337,10 +1342,10 @@
         <v>63</v>
       </c>
       <c r="C64">
-        <v>1.6604000000000001</v>
+        <v>35</v>
       </c>
       <c r="D64">
-        <v>8.3969000000000005</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1351,10 +1356,10 @@
         <v>64</v>
       </c>
       <c r="C65">
-        <v>-0.83190000000000008</v>
+        <v>36</v>
       </c>
       <c r="D65">
-        <v>8.4741999999999997</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1365,10 +1370,10 @@
         <v>65</v>
       </c>
       <c r="C66">
-        <v>0.83180000000000032</v>
+        <v>37</v>
       </c>
       <c r="D66">
-        <v>8.4741999999999997</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1379,10 +1384,892 @@
         <v>66</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="D67">
-        <v>8.5</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <v>41</v>
+      </c>
+      <c r="D68">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <v>42</v>
+      </c>
+      <c r="D69">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <v>35</v>
+      </c>
+      <c r="D70">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <v>38</v>
+      </c>
+      <c r="D71">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <v>39</v>
+      </c>
+      <c r="D72">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <v>34</v>
+      </c>
+      <c r="D73">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <v>41</v>
+      </c>
+      <c r="D74">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <v>42</v>
+      </c>
+      <c r="D75">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76">
+        <v>37</v>
+      </c>
+      <c r="D76">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
+        <v>42</v>
+      </c>
+      <c r="D77">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <v>39</v>
+      </c>
+      <c r="D78">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <v>40</v>
+      </c>
+      <c r="D79">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <v>43</v>
+      </c>
+      <c r="D80">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <v>40</v>
+      </c>
+      <c r="D81">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
+        <v>45</v>
+      </c>
+      <c r="D82">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83">
+        <v>46</v>
+      </c>
+      <c r="D83">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
+        <v>41</v>
+      </c>
+      <c r="D84">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <v>46</v>
+      </c>
+      <c r="D85">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86">
+        <v>49</v>
+      </c>
+      <c r="D86">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87">
+        <v>50</v>
+      </c>
+      <c r="D87">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <v>47</v>
+      </c>
+      <c r="D88">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89">
+        <v>44</v>
+      </c>
+      <c r="D89">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+      <c r="C90">
+        <v>49</v>
+      </c>
+      <c r="D90">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91">
+        <v>50</v>
+      </c>
+      <c r="D91">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92">
+        <v>45</v>
+      </c>
+      <c r="D92">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93">
+        <v>50</v>
+      </c>
+      <c r="D93">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <v>47</v>
+      </c>
+      <c r="D94">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95">
+        <v>48</v>
+      </c>
+      <c r="D95">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96">
+        <v>51</v>
+      </c>
+      <c r="D96">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97">
+        <v>48</v>
+      </c>
+      <c r="D97">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98">
+        <v>53</v>
+      </c>
+      <c r="D98">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99">
+        <v>54</v>
+      </c>
+      <c r="D99">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100">
+        <v>49</v>
+      </c>
+      <c r="D100">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101">
+        <v>54</v>
+      </c>
+      <c r="D101">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>101</v>
+      </c>
+      <c r="C102">
+        <v>59</v>
+      </c>
+      <c r="D102">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>102</v>
+      </c>
+      <c r="C103">
+        <v>60</v>
+      </c>
+      <c r="D103">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>103</v>
+      </c>
+      <c r="C104">
+        <v>55</v>
+      </c>
+      <c r="D104">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>104</v>
+      </c>
+      <c r="C105">
+        <v>52</v>
+      </c>
+      <c r="D105">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>105</v>
+      </c>
+      <c r="C106">
+        <v>59</v>
+      </c>
+      <c r="D106">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>106</v>
+      </c>
+      <c r="C107">
+        <v>60</v>
+      </c>
+      <c r="D107">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>107</v>
+      </c>
+      <c r="C108">
+        <v>53</v>
+      </c>
+      <c r="D108">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>108</v>
+      </c>
+      <c r="C109">
+        <v>60</v>
+      </c>
+      <c r="D109">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>109</v>
+      </c>
+      <c r="C110">
+        <v>57</v>
+      </c>
+      <c r="D110">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>110</v>
+      </c>
+      <c r="C111">
+        <v>56</v>
+      </c>
+      <c r="D111">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>111</v>
+      </c>
+      <c r="C112">
+        <v>55</v>
+      </c>
+      <c r="D112">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>112</v>
+      </c>
+      <c r="C113">
+        <v>56</v>
+      </c>
+      <c r="D113">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>113</v>
+      </c>
+      <c r="C114">
+        <v>61</v>
+      </c>
+      <c r="D114">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>114</v>
+      </c>
+      <c r="C115">
+        <v>58</v>
+      </c>
+      <c r="D115">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>115</v>
+      </c>
+      <c r="C116">
+        <v>62</v>
+      </c>
+      <c r="D116">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>116</v>
+      </c>
+      <c r="C117">
+        <v>63</v>
+      </c>
+      <c r="D117">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>117</v>
+      </c>
+      <c r="C118">
+        <v>64</v>
+      </c>
+      <c r="D118">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>118</v>
+      </c>
+      <c r="C119">
+        <v>65</v>
+      </c>
+      <c r="D119">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>119</v>
+      </c>
+      <c r="C120">
+        <v>59</v>
+      </c>
+      <c r="D120">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>120</v>
+      </c>
+      <c r="C121">
+        <v>63</v>
+      </c>
+      <c r="D121">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>121</v>
+      </c>
+      <c r="C122">
+        <v>64</v>
+      </c>
+      <c r="D122">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>122</v>
+      </c>
+      <c r="C123">
+        <v>65</v>
+      </c>
+      <c r="D123">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>123</v>
+      </c>
+      <c r="C124">
+        <v>64</v>
+      </c>
+      <c r="D124">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>124</v>
+      </c>
+      <c r="C125">
+        <v>65</v>
+      </c>
+      <c r="D125">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>125</v>
+      </c>
+      <c r="C126">
+        <v>66</v>
+      </c>
+      <c r="D126">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>126</v>
+      </c>
+      <c r="C127">
+        <v>62</v>
+      </c>
+      <c r="D127">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>127</v>
+      </c>
+      <c r="C128">
+        <v>65</v>
+      </c>
+      <c r="D128">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>128</v>
+      </c>
+      <c r="C129">
+        <v>64</v>
+      </c>
+      <c r="D129">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>129</v>
+      </c>
+      <c r="C130">
+        <v>66</v>
+      </c>
+      <c r="D130">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1535,8 +2422,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D130"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1544,13 +2431,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1561,10 +2448,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>-7.8</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1575,10 +2462,10 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>-7.4249999999999998</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1589,10 +2476,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>7.4249999999999998</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1603,10 +2490,10 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>7.8</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1617,10 +2504,10 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>-7.8</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1631,10 +2518,10 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>-7.4249999999999998</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1645,10 +2532,10 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>7.4249999999999998</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1659,10 +2546,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>7.8</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1673,10 +2560,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>-7.4265999999999996</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>1.6267</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,10 +2574,10 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>7.4265999999999996</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>1.6267</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1701,10 +2588,10 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>-7.8</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1715,10 +2602,10 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>7.8</v>
       </c>
       <c r="D13">
-        <v>9</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1729,10 +2616,10 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>-7.4281999999999986</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>2.7532999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1743,10 +2630,10 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>7.4281999999999986</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>2.7532999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1757,10 +2644,10 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>-7.8</v>
       </c>
       <c r="D16">
-        <v>11</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1771,10 +2658,10 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>7.8</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1785,10 +2672,10 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>11</v>
+        <v>-7.2062999999999997</v>
       </c>
       <c r="D18">
-        <v>9</v>
+        <v>3.4849000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1799,10 +2686,10 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>7.2062999999999997</v>
       </c>
       <c r="D19">
-        <v>12</v>
+        <v>3.4849000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1813,10 +2700,10 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>-7.8</v>
       </c>
       <c r="D20">
-        <v>13</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1827,10 +2714,10 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>7.8</v>
       </c>
       <c r="D21">
-        <v>14</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,10 +2728,10 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>-6.8459000000000003</v>
       </c>
       <c r="D22">
-        <v>15</v>
+        <v>4.1592000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1855,10 +2742,10 @@
         <v>22</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>6.8458999999999994</v>
       </c>
       <c r="D23">
-        <v>16</v>
+        <v>4.1592000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,10 +2756,10 @@
         <v>23</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>-6.4855</v>
       </c>
       <c r="D24">
-        <v>15</v>
+        <v>4.8334999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1883,10 +2770,10 @@
         <v>24</v>
       </c>
       <c r="C25">
-        <v>12</v>
+        <v>6.4855000000000009</v>
       </c>
       <c r="D25">
-        <v>16</v>
+        <v>4.8334999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1897,10 +2784,10 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>15</v>
+        <v>-7.8</v>
       </c>
       <c r="D26">
-        <v>13</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1911,10 +2798,10 @@
         <v>26</v>
       </c>
       <c r="C27">
-        <v>16</v>
+        <v>7.8</v>
       </c>
       <c r="D27">
-        <v>14</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1925,10 +2812,10 @@
         <v>27</v>
       </c>
       <c r="C28">
-        <v>13</v>
+        <v>-5.9371</v>
       </c>
       <c r="D28">
-        <v>17</v>
+        <v>5.5015999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1939,10 +2826,10 @@
         <v>28</v>
       </c>
       <c r="C29">
-        <v>14</v>
+        <v>5.9371</v>
       </c>
       <c r="D29">
-        <v>18</v>
+        <v>5.5015999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1953,10 +2840,10 @@
         <v>29</v>
       </c>
       <c r="C30">
-        <v>17</v>
+        <v>-7.8</v>
       </c>
       <c r="D30">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1967,10 +2854,10 @@
         <v>30</v>
       </c>
       <c r="C31">
-        <v>18</v>
+        <v>7.8</v>
       </c>
       <c r="D31">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1981,10 +2868,10 @@
         <v>31</v>
       </c>
       <c r="C32">
-        <v>15</v>
+        <v>-5.5153999999999996</v>
       </c>
       <c r="D32">
-        <v>19</v>
+        <v>6.0153999999999996</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1995,10 +2882,10 @@
         <v>32</v>
       </c>
       <c r="C33">
-        <v>16</v>
+        <v>5.5154000000000014</v>
       </c>
       <c r="D33">
-        <v>20</v>
+        <v>6.0153999999999996</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2009,10 +2896,10 @@
         <v>33</v>
       </c>
       <c r="C34">
-        <v>19</v>
+        <v>-4.9851999999999999</v>
       </c>
       <c r="D34">
-        <v>17</v>
+        <v>6.4505999999999997</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2023,10 +2910,10 @@
         <v>34</v>
       </c>
       <c r="C35">
-        <v>20</v>
+        <v>4.9851999999999999</v>
       </c>
       <c r="D35">
-        <v>18</v>
+        <v>6.4505999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2037,10 +2924,10 @@
         <v>35</v>
       </c>
       <c r="C36">
-        <v>21</v>
+        <v>-7.1082000000000001</v>
       </c>
       <c r="D36">
-        <v>17</v>
+        <v>6.4625000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2051,10 +2938,10 @@
         <v>36</v>
       </c>
       <c r="C37">
-        <v>18</v>
+        <v>7.1080999999999994</v>
       </c>
       <c r="D37">
-        <v>22</v>
+        <v>6.4626000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2065,10 +2952,10 @@
         <v>37</v>
       </c>
       <c r="C38">
-        <v>25</v>
+        <v>-6.3889999999999993</v>
       </c>
       <c r="D38">
-        <v>17</v>
+        <v>6.8813000000000004</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2079,10 +2966,10 @@
         <v>38</v>
       </c>
       <c r="C39">
-        <v>26</v>
+        <v>6.3888999999999996</v>
       </c>
       <c r="D39">
-        <v>18</v>
+        <v>6.8814000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2093,10 +2980,10 @@
         <v>39</v>
       </c>
       <c r="C40">
-        <v>23</v>
+        <v>-4.3333999999999993</v>
       </c>
       <c r="D40">
-        <v>21</v>
+        <v>6.9855</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2107,10 +2994,10 @@
         <v>40</v>
       </c>
       <c r="C41">
-        <v>22</v>
+        <v>4.3334000000000001</v>
       </c>
       <c r="D41">
-        <v>24</v>
+        <v>6.9855</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2121,10 +3008,10 @@
         <v>41</v>
       </c>
       <c r="C42">
-        <v>19</v>
+        <v>-5.6452</v>
       </c>
       <c r="D42">
-        <v>25</v>
+        <v>7.2546999999999997</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2135,10 +3022,10 @@
         <v>42</v>
       </c>
       <c r="C43">
-        <v>20</v>
+        <v>5.6451000000000002</v>
       </c>
       <c r="D43">
-        <v>26</v>
+        <v>7.2546999999999997</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2149,10 +3036,10 @@
         <v>43</v>
       </c>
       <c r="C44">
-        <v>25</v>
+        <v>-3.7848000000000002</v>
       </c>
       <c r="D44">
-        <v>21</v>
+        <v>7.2786999999999997</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2163,10 +3050,10 @@
         <v>44</v>
       </c>
       <c r="C45">
-        <v>26</v>
+        <v>3.7848000000000002</v>
       </c>
       <c r="D45">
-        <v>22</v>
+        <v>7.2786999999999997</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2177,10 +3064,10 @@
         <v>45</v>
       </c>
       <c r="C46">
-        <v>25</v>
+        <v>-4.8796999999999997</v>
       </c>
       <c r="D46">
-        <v>23</v>
+        <v>7.5812999999999997</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2191,10 +3078,10 @@
         <v>46</v>
       </c>
       <c r="C47">
-        <v>24</v>
+        <v>4.8796000000000008</v>
       </c>
       <c r="D47">
-        <v>26</v>
+        <v>7.5812999999999997</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2205,10 +3092,10 @@
         <v>47</v>
       </c>
       <c r="C48">
-        <v>27</v>
+        <v>-2.9849000000000001</v>
       </c>
       <c r="D48">
-        <v>23</v>
+        <v>7.7062999999999997</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2219,10 +3106,10 @@
         <v>48</v>
       </c>
       <c r="C49">
-        <v>24</v>
+        <v>2.984900000000001</v>
       </c>
       <c r="D49">
-        <v>28</v>
+        <v>7.7062999999999997</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2233,10 +3120,10 @@
         <v>49</v>
       </c>
       <c r="C50">
-        <v>29</v>
+        <v>-4.0953999999999997</v>
       </c>
       <c r="D50">
-        <v>23</v>
+        <v>7.8597000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2247,10 +3134,10 @@
         <v>50</v>
       </c>
       <c r="C51">
-        <v>30</v>
+        <v>4.0954000000000006</v>
       </c>
       <c r="D51">
-        <v>24</v>
+        <v>7.8597000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2261,10 +3148,10 @@
         <v>51</v>
       </c>
       <c r="C52">
-        <v>25</v>
+        <v>-2.3689</v>
       </c>
       <c r="D52">
-        <v>29</v>
+        <v>7.8930999999999996</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2275,10 +3162,10 @@
         <v>52</v>
       </c>
       <c r="C53">
-        <v>26</v>
+        <v>2.3689000000000009</v>
       </c>
       <c r="D53">
-        <v>30</v>
+        <v>7.8930999999999996</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2289,10 +3176,10 @@
         <v>53</v>
       </c>
       <c r="C54">
-        <v>35</v>
+        <v>-3.2953999999999999</v>
       </c>
       <c r="D54">
-        <v>23</v>
+        <v>8.0890000000000004</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2303,10 +3190,10 @@
         <v>54</v>
       </c>
       <c r="C55">
-        <v>36</v>
+        <v>3.2953999999999999</v>
       </c>
       <c r="D55">
-        <v>24</v>
+        <v>8.0891000000000002</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2317,10 +3204,10 @@
         <v>55</v>
       </c>
       <c r="C56">
-        <v>31</v>
+        <v>-1.5217000000000001</v>
       </c>
       <c r="D56">
-        <v>27</v>
+        <v>8.1501000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2331,10 +3218,10 @@
         <v>56</v>
       </c>
       <c r="C57">
-        <v>28</v>
+        <v>1.5217000000000001</v>
       </c>
       <c r="D57">
-        <v>32</v>
+        <v>8.1501000000000001</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2345,10 +3232,10 @@
         <v>57</v>
       </c>
       <c r="C58">
-        <v>35</v>
+        <v>-0.80679999999999996</v>
       </c>
       <c r="D58">
-        <v>27</v>
+        <v>8.2204999999999995</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2359,10 +3246,10 @@
         <v>58</v>
       </c>
       <c r="C59">
-        <v>36</v>
+        <v>0.80679999999999996</v>
       </c>
       <c r="D59">
-        <v>28</v>
+        <v>8.2204999999999995</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2373,10 +3260,10 @@
         <v>59</v>
       </c>
       <c r="C60">
-        <v>29</v>
+        <v>-2.482699999999999</v>
       </c>
       <c r="D60">
-        <v>35</v>
+        <v>8.2683</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2387,10 +3274,10 @@
         <v>60</v>
       </c>
       <c r="C61">
-        <v>36</v>
+        <v>2.4826999999999999</v>
       </c>
       <c r="D61">
-        <v>30</v>
+        <v>8.2683</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2401,10 +3288,10 @@
         <v>61</v>
       </c>
       <c r="C62">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>31</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2415,10 +3302,10 @@
         <v>62</v>
       </c>
       <c r="C63">
-        <v>32</v>
+        <v>-1.6605000000000001</v>
       </c>
       <c r="D63">
-        <v>34</v>
+        <v>8.3969000000000005</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2429,10 +3316,10 @@
         <v>63</v>
       </c>
       <c r="C64">
-        <v>35</v>
+        <v>1.6604000000000001</v>
       </c>
       <c r="D64">
-        <v>31</v>
+        <v>8.3969000000000005</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2443,10 +3330,10 @@
         <v>64</v>
       </c>
       <c r="C65">
-        <v>36</v>
+        <v>-0.83190000000000008</v>
       </c>
       <c r="D65">
-        <v>32</v>
+        <v>8.4741999999999997</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2457,10 +3344,10 @@
         <v>65</v>
       </c>
       <c r="C66">
-        <v>37</v>
+        <v>0.83180000000000032</v>
       </c>
       <c r="D66">
-        <v>31</v>
+        <v>8.4741999999999997</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2471,892 +3358,10 @@
         <v>66</v>
       </c>
       <c r="C67">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>67</v>
-      </c>
-      <c r="B68">
-        <v>67</v>
-      </c>
-      <c r="C68">
-        <v>41</v>
-      </c>
-      <c r="D68">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>68</v>
-      </c>
-      <c r="B69">
-        <v>68</v>
-      </c>
-      <c r="C69">
-        <v>42</v>
-      </c>
-      <c r="D69">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>69</v>
-      </c>
-      <c r="B70">
-        <v>69</v>
-      </c>
-      <c r="C70">
-        <v>35</v>
-      </c>
-      <c r="D70">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>70</v>
-      </c>
-      <c r="B71">
-        <v>70</v>
-      </c>
-      <c r="C71">
-        <v>38</v>
-      </c>
-      <c r="D71">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>71</v>
-      </c>
-      <c r="B72">
-        <v>71</v>
-      </c>
-      <c r="C72">
-        <v>39</v>
-      </c>
-      <c r="D72">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>72</v>
-      </c>
-      <c r="B73">
-        <v>72</v>
-      </c>
-      <c r="C73">
-        <v>34</v>
-      </c>
-      <c r="D73">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <v>73</v>
-      </c>
-      <c r="C74">
-        <v>41</v>
-      </c>
-      <c r="D74">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>74</v>
-      </c>
-      <c r="B75">
-        <v>74</v>
-      </c>
-      <c r="C75">
-        <v>42</v>
-      </c>
-      <c r="D75">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>75</v>
-      </c>
-      <c r="B76">
-        <v>75</v>
-      </c>
-      <c r="C76">
-        <v>37</v>
-      </c>
-      <c r="D76">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>76</v>
-      </c>
-      <c r="B77">
-        <v>76</v>
-      </c>
-      <c r="C77">
-        <v>42</v>
-      </c>
-      <c r="D77">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>77</v>
-      </c>
-      <c r="B78">
-        <v>77</v>
-      </c>
-      <c r="C78">
-        <v>39</v>
-      </c>
-      <c r="D78">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>78</v>
-      </c>
-      <c r="B79">
-        <v>78</v>
-      </c>
-      <c r="C79">
-        <v>40</v>
-      </c>
-      <c r="D79">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <v>79</v>
-      </c>
-      <c r="B80">
-        <v>79</v>
-      </c>
-      <c r="C80">
-        <v>43</v>
-      </c>
-      <c r="D80">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>80</v>
-      </c>
-      <c r="B81">
-        <v>80</v>
-      </c>
-      <c r="C81">
-        <v>40</v>
-      </c>
-      <c r="D81">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>81</v>
-      </c>
-      <c r="B82">
-        <v>81</v>
-      </c>
-      <c r="C82">
-        <v>45</v>
-      </c>
-      <c r="D82">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>82</v>
-      </c>
-      <c r="B83">
-        <v>82</v>
-      </c>
-      <c r="C83">
-        <v>46</v>
-      </c>
-      <c r="D83">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>83</v>
-      </c>
-      <c r="B84">
-        <v>83</v>
-      </c>
-      <c r="C84">
-        <v>41</v>
-      </c>
-      <c r="D84">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>84</v>
-      </c>
-      <c r="B85">
-        <v>84</v>
-      </c>
-      <c r="C85">
-        <v>46</v>
-      </c>
-      <c r="D85">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>85</v>
-      </c>
-      <c r="B86">
-        <v>85</v>
-      </c>
-      <c r="C86">
-        <v>49</v>
-      </c>
-      <c r="D86">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <v>86</v>
-      </c>
-      <c r="B87">
-        <v>86</v>
-      </c>
-      <c r="C87">
-        <v>50</v>
-      </c>
-      <c r="D87">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>87</v>
-      </c>
-      <c r="B88">
-        <v>87</v>
-      </c>
-      <c r="C88">
-        <v>47</v>
-      </c>
-      <c r="D88">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>88</v>
-      </c>
-      <c r="B89">
-        <v>88</v>
-      </c>
-      <c r="C89">
-        <v>44</v>
-      </c>
-      <c r="D89">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <v>89</v>
-      </c>
-      <c r="B90">
-        <v>89</v>
-      </c>
-      <c r="C90">
-        <v>49</v>
-      </c>
-      <c r="D90">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>90</v>
-      </c>
-      <c r="B91">
-        <v>90</v>
-      </c>
-      <c r="C91">
-        <v>50</v>
-      </c>
-      <c r="D91">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>91</v>
-      </c>
-      <c r="B92">
-        <v>91</v>
-      </c>
-      <c r="C92">
-        <v>45</v>
-      </c>
-      <c r="D92">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <v>92</v>
-      </c>
-      <c r="B93">
-        <v>92</v>
-      </c>
-      <c r="C93">
-        <v>50</v>
-      </c>
-      <c r="D93">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <v>93</v>
-      </c>
-      <c r="B94">
-        <v>93</v>
-      </c>
-      <c r="C94">
-        <v>47</v>
-      </c>
-      <c r="D94">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <v>94</v>
-      </c>
-      <c r="B95">
-        <v>94</v>
-      </c>
-      <c r="C95">
-        <v>48</v>
-      </c>
-      <c r="D95">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>95</v>
-      </c>
-      <c r="B96">
-        <v>95</v>
-      </c>
-      <c r="C96">
-        <v>51</v>
-      </c>
-      <c r="D96">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>96</v>
-      </c>
-      <c r="B97">
-        <v>96</v>
-      </c>
-      <c r="C97">
-        <v>48</v>
-      </c>
-      <c r="D97">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>97</v>
-      </c>
-      <c r="B98">
-        <v>97</v>
-      </c>
-      <c r="C98">
-        <v>53</v>
-      </c>
-      <c r="D98">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>98</v>
-      </c>
-      <c r="B99">
-        <v>98</v>
-      </c>
-      <c r="C99">
-        <v>54</v>
-      </c>
-      <c r="D99">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>99</v>
-      </c>
-      <c r="B100">
-        <v>99</v>
-      </c>
-      <c r="C100">
-        <v>49</v>
-      </c>
-      <c r="D100">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>100</v>
-      </c>
-      <c r="B101">
-        <v>100</v>
-      </c>
-      <c r="C101">
-        <v>54</v>
-      </c>
-      <c r="D101">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>101</v>
-      </c>
-      <c r="B102">
-        <v>101</v>
-      </c>
-      <c r="C102">
-        <v>59</v>
-      </c>
-      <c r="D102">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>102</v>
-      </c>
-      <c r="B103">
-        <v>102</v>
-      </c>
-      <c r="C103">
-        <v>60</v>
-      </c>
-      <c r="D103">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <v>103</v>
-      </c>
-      <c r="B104">
-        <v>103</v>
-      </c>
-      <c r="C104">
-        <v>55</v>
-      </c>
-      <c r="D104">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>104</v>
-      </c>
-      <c r="B105">
-        <v>104</v>
-      </c>
-      <c r="C105">
-        <v>52</v>
-      </c>
-      <c r="D105">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>105</v>
-      </c>
-      <c r="B106">
-        <v>105</v>
-      </c>
-      <c r="C106">
-        <v>59</v>
-      </c>
-      <c r="D106">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>106</v>
-      </c>
-      <c r="B107">
-        <v>106</v>
-      </c>
-      <c r="C107">
-        <v>60</v>
-      </c>
-      <c r="D107">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
-        <v>107</v>
-      </c>
-      <c r="B108">
-        <v>107</v>
-      </c>
-      <c r="C108">
-        <v>53</v>
-      </c>
-      <c r="D108">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
-        <v>108</v>
-      </c>
-      <c r="B109">
-        <v>108</v>
-      </c>
-      <c r="C109">
-        <v>60</v>
-      </c>
-      <c r="D109">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <v>109</v>
-      </c>
-      <c r="B110">
-        <v>109</v>
-      </c>
-      <c r="C110">
-        <v>57</v>
-      </c>
-      <c r="D110">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>110</v>
-      </c>
-      <c r="B111">
-        <v>110</v>
-      </c>
-      <c r="C111">
-        <v>56</v>
-      </c>
-      <c r="D111">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>111</v>
-      </c>
-      <c r="B112">
-        <v>111</v>
-      </c>
-      <c r="C112">
-        <v>55</v>
-      </c>
-      <c r="D112">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <v>112</v>
-      </c>
-      <c r="B113">
-        <v>112</v>
-      </c>
-      <c r="C113">
-        <v>56</v>
-      </c>
-      <c r="D113">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <v>113</v>
-      </c>
-      <c r="B114">
-        <v>113</v>
-      </c>
-      <c r="C114">
-        <v>61</v>
-      </c>
-      <c r="D114">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <v>114</v>
-      </c>
-      <c r="B115">
-        <v>114</v>
-      </c>
-      <c r="C115">
-        <v>58</v>
-      </c>
-      <c r="D115">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>115</v>
-      </c>
-      <c r="B116">
-        <v>115</v>
-      </c>
-      <c r="C116">
-        <v>62</v>
-      </c>
-      <c r="D116">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>116</v>
-      </c>
-      <c r="B117">
-        <v>116</v>
-      </c>
-      <c r="C117">
-        <v>63</v>
-      </c>
-      <c r="D117">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <v>117</v>
-      </c>
-      <c r="B118">
-        <v>117</v>
-      </c>
-      <c r="C118">
-        <v>64</v>
-      </c>
-      <c r="D118">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>118</v>
-      </c>
-      <c r="B119">
-        <v>118</v>
-      </c>
-      <c r="C119">
-        <v>65</v>
-      </c>
-      <c r="D119">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>119</v>
-      </c>
-      <c r="B120">
-        <v>119</v>
-      </c>
-      <c r="C120">
-        <v>59</v>
-      </c>
-      <c r="D120">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
-        <v>120</v>
-      </c>
-      <c r="B121">
-        <v>120</v>
-      </c>
-      <c r="C121">
-        <v>63</v>
-      </c>
-      <c r="D121">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>121</v>
-      </c>
-      <c r="B122">
-        <v>121</v>
-      </c>
-      <c r="C122">
-        <v>64</v>
-      </c>
-      <c r="D122">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
-        <v>122</v>
-      </c>
-      <c r="B123">
-        <v>122</v>
-      </c>
-      <c r="C123">
-        <v>65</v>
-      </c>
-      <c r="D123">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
-        <v>123</v>
-      </c>
-      <c r="B124">
-        <v>123</v>
-      </c>
-      <c r="C124">
-        <v>64</v>
-      </c>
-      <c r="D124">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
-        <v>124</v>
-      </c>
-      <c r="B125">
-        <v>124</v>
-      </c>
-      <c r="C125">
-        <v>65</v>
-      </c>
-      <c r="D125">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
-        <v>125</v>
-      </c>
-      <c r="B126">
-        <v>125</v>
-      </c>
-      <c r="C126">
-        <v>66</v>
-      </c>
-      <c r="D126">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
-        <v>126</v>
-      </c>
-      <c r="B127">
-        <v>126</v>
-      </c>
-      <c r="C127">
-        <v>62</v>
-      </c>
-      <c r="D127">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
-        <v>127</v>
-      </c>
-      <c r="B128">
-        <v>127</v>
-      </c>
-      <c r="C128">
-        <v>65</v>
-      </c>
-      <c r="D128">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <v>128</v>
-      </c>
-      <c r="B129">
-        <v>128</v>
-      </c>
-      <c r="C129">
-        <v>64</v>
-      </c>
-      <c r="D129">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
-        <v>129</v>
-      </c>
-      <c r="B130">
-        <v>129</v>
-      </c>
-      <c r="C130">
-        <v>66</v>
-      </c>
-      <c r="D130">
-        <v>65</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -5250,8 +5255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5266,7 +5271,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5274,7 +5279,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5282,12 +5287,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5327,13 +5335,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="B1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5342,370 +5352,6 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>29</v>
-      </c>
-      <c r="C2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D2">
-        <v>13.95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>35</v>
-      </c>
-      <c r="C3">
-        <v>-14.59</v>
-      </c>
-      <c r="D3">
-        <v>13.26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>37</v>
-      </c>
-      <c r="C4">
-        <v>-11.37</v>
-      </c>
-      <c r="D4">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>41</v>
-      </c>
-      <c r="C5">
-        <v>-8.5299999999999994</v>
-      </c>
-      <c r="D5">
-        <v>10.96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>45</v>
-      </c>
-      <c r="C6">
-        <v>-6.1</v>
-      </c>
-      <c r="D6">
-        <v>9.4700000000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>49</v>
-      </c>
-      <c r="C7">
-        <v>-4.08</v>
-      </c>
-      <c r="D7">
-        <v>7.83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>53</v>
-      </c>
-      <c r="C8">
-        <v>-2.5</v>
-      </c>
-      <c r="D8">
-        <v>6.13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>59</v>
-      </c>
-      <c r="C9">
-        <v>-1.23</v>
-      </c>
-      <c r="D9">
-        <v>4.09</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>62</v>
-      </c>
-      <c r="C10">
-        <v>-0.51</v>
-      </c>
-      <c r="D10">
-        <v>2.57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>64</v>
-      </c>
-      <c r="C11">
-        <v>-0.12</v>
-      </c>
-      <c r="D11">
-        <v>1.19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>66</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>65</v>
-      </c>
-      <c r="C13">
-        <v>0.11</v>
-      </c>
-      <c r="D13">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>63</v>
-      </c>
-      <c r="C14">
-        <v>0.42</v>
-      </c>
-      <c r="D14">
-        <v>2.14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>60</v>
-      </c>
-      <c r="C15">
-        <v>0.9</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>54</v>
-      </c>
-      <c r="C16">
-        <v>1.5</v>
-      </c>
-      <c r="D16">
-        <v>3.68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>2.19</v>
-      </c>
-      <c r="D17">
-        <v>4.1900000000000004</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>46</v>
-      </c>
-      <c r="C18">
-        <v>2.92</v>
-      </c>
-      <c r="D18">
-        <v>4.54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>42</v>
-      </c>
-      <c r="C19">
-        <v>3.67</v>
-      </c>
-      <c r="D19">
-        <v>4.71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>38</v>
-      </c>
-      <c r="C20">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D20">
-        <v>4.74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>36</v>
-      </c>
-      <c r="C21">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D21">
-        <v>4.6399999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>30</v>
-      </c>
-      <c r="C22">
-        <v>5.74</v>
-      </c>
-      <c r="D22">
-        <v>4.42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23">
-        <v>6.5469999999999997</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>11</v>
-      </c>
-      <c r="C24">
-        <v>13.551</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>15</v>
-      </c>
-      <c r="C25">
-        <v>20.555</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>19</v>
-      </c>
-      <c r="C26">
-        <v>27.559000000000001</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>25</v>
-      </c>
-      <c r="C27">
-        <v>33.802</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5715,9 +5361,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5740,10 +5388,10 @@
         <v>29</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D2">
-        <v>-1.33</v>
+        <v>13.95</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5751,13 +5399,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-14.59</v>
       </c>
       <c r="D3">
-        <v>-1.33</v>
+        <v>13.26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5765,13 +5413,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-11.37</v>
       </c>
       <c r="D4">
-        <v>-1.33</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5779,13 +5427,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-8.5299999999999994</v>
       </c>
       <c r="D5">
-        <v>-1.33</v>
+        <v>10.96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5793,13 +5441,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>-6.1</v>
       </c>
       <c r="D6">
-        <v>-1.33</v>
+        <v>9.4700000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5807,13 +5455,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>-4.08</v>
       </c>
       <c r="D7">
-        <v>-1.33</v>
+        <v>7.83</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5821,13 +5469,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="D8">
-        <v>-1.33</v>
+        <v>6.13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5835,13 +5483,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>-1.23</v>
       </c>
       <c r="D9">
-        <v>-1.33</v>
+        <v>4.09</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5849,13 +5497,13 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>-0.51</v>
       </c>
       <c r="D10">
-        <v>-1.33</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5863,13 +5511,13 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>-0.12</v>
       </c>
       <c r="D11">
-        <v>-1.33</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5877,13 +5525,13 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>-1.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5891,13 +5539,13 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="D13">
-        <v>-1.33</v>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5905,13 +5553,13 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="D14">
-        <v>-1.33</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5919,13 +5567,13 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D15">
-        <v>-1.33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5933,13 +5581,13 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D16">
-        <v>-1.33</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5947,13 +5595,13 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>2.19</v>
       </c>
       <c r="D17">
-        <v>-1.33</v>
+        <v>4.1900000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5961,13 +5609,13 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>2.92</v>
       </c>
       <c r="D18">
-        <v>-1.33</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5975,13 +5623,13 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>3.67</v>
       </c>
       <c r="D19">
-        <v>-1.33</v>
+        <v>4.71</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5989,13 +5637,13 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D20">
-        <v>-1.33</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -6003,13 +5651,13 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D21">
-        <v>-1.33</v>
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -6017,13 +5665,83 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>5.74</v>
       </c>
       <c r="D22">
-        <v>-1.33</v>
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>6.5469999999999997</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>13.551</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>20.555</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>27.559000000000001</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>33.802</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6035,7 +5753,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6061,7 +5781,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6075,7 +5795,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6089,7 +5809,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6103,7 +5823,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6117,7 +5837,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6131,7 +5851,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6145,7 +5865,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6159,7 +5879,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6173,7 +5893,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6187,7 +5907,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6201,7 +5921,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6215,7 +5935,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6229,7 +5949,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -6243,7 +5963,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6257,7 +5977,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -6271,7 +5991,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -6285,7 +6005,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -6299,7 +6019,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -6313,7 +6033,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -6327,7 +6047,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -6341,7 +6061,7 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>-2.66</v>
+        <v>-1.33</v>
       </c>
     </row>
   </sheetData>
@@ -6351,13 +6071,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6366,6 +6088,300 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>42</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>49</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>53</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>54</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>59</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>62</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>63</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>64</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>65</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>-2.66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>66</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>-2.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>